<commit_message>
73600-Summary of FM35 funding report - excel version
</commit_message>
<xml_diff>
--- a/src/ESFA.DC.ILR.ReportService.Service/Reports/Templates/SummaryOfFM35FundingTemplate.xlsx
+++ b/src/ESFA.DC.ILR.ReportService.Service/Reports/Templates/SummaryOfFM35FundingTemplate.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gayatri\source\repos\DC-ILR-1819-ReportService\src\ESFA.DC.ILR.ReportService.Service\Reports\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51E0F605-EAB8-4038-AFA3-0D663162DFF3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53F79DF6-00B4-4927-9A20-B53D4A38F069}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{800BCD35-0AED-48A0-B854-F52B11BD9E58}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Summary of FM35 Funding Report" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
   <si>
     <t>Funding Line Type</t>
   </si>
@@ -54,13 +54,64 @@
   </si>
   <si>
     <t>Provider specified learning delivery data (D)</t>
+  </si>
+  <si>
+    <t>Period</t>
+  </si>
+  <si>
+    <t>On Programme (£)</t>
+  </si>
+  <si>
+    <t>Balancing (£)</t>
+  </si>
+  <si>
+    <t>Job Outcome Achievement (£)</t>
+  </si>
+  <si>
+    <t>Aim Achievement (£)</t>
+  </si>
+  <si>
+    <t>Total Achievement (£)</t>
+  </si>
+  <si>
+    <t>Learning Support (£)</t>
+  </si>
+  <si>
+    <t>Total (£)</t>
+  </si>
+  <si>
+    <t>&amp;=GroupedModels.Period</t>
+  </si>
+  <si>
+    <t>&amp;=GroupedModels.OnProgramme</t>
+  </si>
+  <si>
+    <t>&amp;=GroupedModels.Balancing</t>
+  </si>
+  <si>
+    <t>&amp;=GroupedModels.JobOutcomeAchievement</t>
+  </si>
+  <si>
+    <t>&amp;=GroupedModels.AimAchievement</t>
+  </si>
+  <si>
+    <t>&amp;=GroupedModels.TotalAchievement</t>
+  </si>
+  <si>
+    <t>&amp;=GroupedModels.LearningSupport</t>
+  </si>
+  <si>
+    <t>&amp;=GroupedModels.Total</t>
+  </si>
+  <si>
+    <t>&amp;=GroupedModels.FundingLineType</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -87,6 +138,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -96,7 +154,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -104,11 +162,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -119,6 +192,15 @@
       <alignment wrapText="1" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -437,13 +519,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49500DBD-B2AE-434D-9770-C90E73E373EA}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:I25"/>
+  <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -455,57 +534,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7"/>
+      <c r="B1" s="10"/>
       <c r="C1" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D1" s="3"/>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
       <c r="H1" s="3" t="s">
         <v>3</v>
       </c>
       <c r="I1" s="3"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="7"/>
+      <c r="B2" s="10"/>
       <c r="C2" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="3"/>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
       <c r="H2" s="3" t="s">
         <v>3</v>
       </c>
       <c r="I2" s="3"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="7"/>
+      <c r="B3" s="10"/>
       <c r="C3" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D3" s="3"/>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
       <c r="H3" s="3" t="s">
         <v>3</v>
       </c>
@@ -516,37 +595,73 @@
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
       <c r="H4" s="3" t="s">
         <v>3</v>
       </c>
       <c r="I4" s="3"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
+    <row r="6" spans="1:9" ht="33.75" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="33.75" x14ac:dyDescent="0.2">
+      <c r="A7" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="I7" s="8" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="5"/>
@@ -626,48 +741,48 @@
       <c r="I14" s="5"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
+      <c r="A15" s="5"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
+      <c r="A16" s="5"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
+      <c r="A17" s="5"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="2"/>
@@ -745,6 +860,39 @@
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" s="2"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A27" s="2"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A28" s="2"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -759,10 +907,7 @@
   <pageMargins left="0.7" right="0.7" top="1.5" bottom="1.5" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
   <headerFooter>
-    <oddHeader>&amp;L&amp;"Arial,Regular"&amp;16Summary of Funding Model 35 Funding
-&amp;"Arial,Bold"&amp;10Provider:
-UKPRN:
-ILR File:&amp;R&amp;"Arial,Bold"&amp;10OFFICIAL-SENSITIVE</oddHeader>
+    <oddHeader>&amp;L&amp;"Arial,Regular"&amp;16Summary of Funding Model 35 Funding&amp;R&amp;"Arial,Bold"&amp;10OFFICIAL-SENSITIVE</oddHeader>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>